<commit_message>
Finished first version of DA for Campanian case with Kristianstad data
</commit_message>
<xml_diff>
--- a/Campanian case/Kristianstad_seasonal_data.xlsx
+++ b/Campanian case/Kristianstad_seasonal_data.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Side projects\Bayesian temperature models\Seasonal DA\SeasonalDA_script\Campanian case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C0C2C9D2-986E-42A5-8006-71611AC3CF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75404D68-73B2-4D68-A85B-6056D49D7A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22725" yWindow="1920" windowWidth="21600" windowHeight="12030" xr2:uid="{337FB45E-1141-4D61-A5E0-6D30CD15E1C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{337FB45E-1141-4D61-A5E0-6D30CD15E1C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Kristianstad_seasonal_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Month</t>
   </si>
@@ -65,6 +78,24 @@
   </si>
   <si>
     <t>Month_align2</t>
+  </si>
+  <si>
+    <t>d18Oc_median</t>
+  </si>
+  <si>
+    <t>d18Oc_SE</t>
+  </si>
+  <si>
+    <t>d18Oc_SE_Tmin</t>
+  </si>
+  <si>
+    <t>d18Oc_SE_Tmax</t>
+  </si>
+  <si>
+    <t>d18Oc_SE_dwmin</t>
+  </si>
+  <si>
+    <t>d18Oc_SE_dwmax</t>
   </si>
 </sst>
 </file>
@@ -925,15 +956,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307904F0-873C-4D31-B897-C59C733CDF53}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,10 +1015,28 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1008,11 +1073,35 @@
       <c r="K2">
         <v>0.171038151</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <f>((EXP(((18.03 * 10 ^ 3) / (F2 + 273.15) - 32.42) / 1000) * (((I2 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-2.1048140983096486</v>
+      </c>
+      <c r="M2">
+        <f>((EXP(((18.03 * 10 ^ 3) / (F2 - H2 + 273.15) - 32.42) / 1000) * (((I2 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-1.8999217866088047</v>
+      </c>
+      <c r="N2">
+        <f>((EXP(((18.03 * 10 ^ 3) / (F2 + H2 + 273.15) - 32.42) / 1000) * (((I2 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-2.3082673984518021</v>
+      </c>
+      <c r="O2">
+        <f>((EXP(((18.03 * 10 ^ 3) / (F2 + 273.15) - 32.42) / 1000) * (((I2 - K2 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-2.275326848430459</v>
+      </c>
+      <c r="P2">
+        <f>((EXP(((18.03 * 10 ^ 3) / (F2 + 273.15) - 32.42) / 1000) * (((I2 + K2 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-1.9343013481888383</v>
+      </c>
+      <c r="Q2">
+        <f>SQRT((M2-N2)^2 + (O2-P2)^2)</f>
+        <v>0.53201929525768099</v>
+      </c>
+      <c r="R2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1025,7 +1114,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D14" si="2">IF(MOD(A3+3, 12)=0, 12, MOD(A3+3, 12))</f>
+        <f t="shared" ref="D3:D13" si="2">IF(MOD(A3+3, 12)=0, 12, MOD(A3+3, 12))</f>
         <v>5</v>
       </c>
       <c r="E3">
@@ -1049,11 +1138,35 @@
       <c r="K3">
         <v>0.25216394199999997</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <f t="shared" ref="L3:L37" si="3">((EXP(((18.03 * 10 ^ 3) / (F3 + 273.15) - 32.42) / 1000) * (((I3 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-2.2172773717509253</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M37" si="4">((EXP(((18.03 * 10 ^ 3) / (F3 - H3 + 273.15) - 32.42) / 1000) * (((I3 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-1.8724731985750864</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N37" si="5">((EXP(((18.03 * 10 ^ 3) / (F3 + H3 + 273.15) - 32.42) / 1000) * (((I3 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-2.5580172565763393</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O37" si="6">((EXP(((18.03 * 10 ^ 3) / (F3 + 273.15) - 32.42) / 1000) * (((I3 - K3 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-2.4686358650249929</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P37" si="7">((EXP(((18.03 * 10 ^ 3) / (F3 + 273.15) - 32.42) / 1000) * (((I3 + K3 - 30.92) / 1.03092) / 1000 + 1)) - 1) * 1000</f>
+        <v>-1.9659188784768578</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q37" si="8">SQRT((M3-N3)^2 + (O3-P3)^2)</f>
+        <v>0.85011471227409241</v>
+      </c>
+      <c r="R3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1090,11 +1203,35 @@
       <c r="K4">
         <v>0.19862494999999999</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>-2.1569847877871418</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>-1.906155450812963</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>-2.4056551666112869</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="6"/>
+        <v>-2.3549674854781433</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="7"/>
+        <v>-1.9590020900963623</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="8"/>
+        <v>0.6374076877654179</v>
+      </c>
+      <c r="R4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1131,11 +1268,35 @@
       <c r="K5">
         <v>0.17393377300000001</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>-2.1551418061938055</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>-1.9400377576505035</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>-2.3686564533154097</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>-2.3285152176978352</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="7"/>
+        <v>-1.9817683946898867</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="8"/>
+        <v>0.55131419856520214</v>
+      </c>
+      <c r="R5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1172,11 +1333,35 @@
       <c r="K6">
         <v>0.16271224000000001</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>-1.8735312502722312</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>-1.6608081153225429</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="5"/>
+        <v>-2.0847152498323362</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>-2.0358169295462414</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="7"/>
+        <v>-1.71124557099811</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="8"/>
+        <v>0.53389495734468562</v>
+      </c>
+      <c r="R6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1213,11 +1398,35 @@
       <c r="K7">
         <v>0.12294068800000001</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>-1.6675794885263606</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>-1.4963302924599908</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>-1.8378370853633363</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>-1.7902525998699792</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="7"/>
+        <v>-1.544906377182742</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="8"/>
+        <v>0.42050167489086637</v>
+      </c>
+      <c r="R7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1254,11 +1463,35 @@
       <c r="K8">
         <v>0.12329092</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>-1.3507833562019789</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>-1.1887312256657623</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>-1.511956859944652</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>-1.4738880401297116</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="7"/>
+        <v>-1.2276786722740241</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="8"/>
+        <v>0.40631744175568918</v>
+      </c>
+      <c r="R8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1295,11 +1528,35 @@
       <c r="K9">
         <v>0.15723779800000001</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>-1.2887010881212912</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>-1.0689171646183215</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>-1.5068776618868407</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>-1.4457362536000051</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="7"/>
+        <v>-1.1316659226426884</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="8"/>
+        <v>0.53893373428959435</v>
+      </c>
+      <c r="R9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1336,11 +1593,35 @@
       <c r="K10">
         <v>0.15851689799999999</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>-1.3126911201369884</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>-1.0793304097548306</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>-1.5442381575627717</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>-1.4709904364537119</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
+        <v>-1.154391803820487</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="8"/>
+        <v>0.56247125096050898</v>
+      </c>
+      <c r="R10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1377,11 +1658,35 @@
       <c r="K11">
         <v>0.179280619</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>-1.3833264222030683</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>-1.1222204151511983</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>-1.6421566400643961</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>-1.5623250278508083</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="7"/>
+        <v>-1.2043278165554394</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="8"/>
+        <v>0.63126514340033735</v>
+      </c>
+      <c r="R11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1418,11 +1723,35 @@
       <c r="K12">
         <v>0.171130281</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>-1.6657129987237562</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>-1.419698881572895</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>-1.9096884848486262</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>-1.8364847939182916</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="7"/>
+        <v>-1.4949412035291099</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="8"/>
+        <v>0.59727869161241764</v>
+      </c>
+      <c r="R12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1459,11 +1788,35 @@
       <c r="K13">
         <v>0.16940219200000001</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>-1.7028428261518513</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>-1.4686223757985895</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>-1.9352102978147379</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>-1.8718652807189207</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="7"/>
+        <v>-1.533820371584671</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="8"/>
+        <v>0.57617588422540778</v>
+      </c>
+      <c r="R13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1500,24 +1853,48 @@
       <c r="K14">
         <v>0.100693141</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>-1.0093840460483339</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>-0.8129422103710926</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>-1.2045623245275916</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>-1.1100550791144359</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="7"/>
+        <v>-0.90871301298234286</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="8"/>
+        <v>0.4403463879791561</v>
+      </c>
+      <c r="R14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:B25" si="3">IF(MOD(A15+1, 12)=0, 12, MOD(A15+1, 12))</f>
+        <f t="shared" ref="B15:B25" si="9">IF(MOD(A15+1, 12)=0, 12, MOD(A15+1, 12))</f>
         <v>3</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C25" si="4">IF(MOD(A15, 12)=0, 12, MOD(A15, 12))</f>
+        <f t="shared" ref="C15:C25" si="10">IF(MOD(A15, 12)=0, 12, MOD(A15, 12))</f>
         <v>2</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D26" si="5">IF(MOD(A15-1, 12)=0, 12, MOD(A15-1, 12))</f>
+        <f t="shared" ref="D15:D25" si="11">IF(MOD(A15-1, 12)=0, 12, MOD(A15-1, 12))</f>
         <v>1</v>
       </c>
       <c r="E15">
@@ -1541,24 +1918,48 @@
       <c r="K15">
         <v>0.104364873</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>-0.87139399151769936</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>-0.71596201858892261</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>-1.0260368467880365</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>-0.97576080806116572</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="7"/>
+        <v>-0.76702717497423301</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="8"/>
+        <v>0.37378620716176819</v>
+      </c>
+      <c r="R15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="C16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="D16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="E16">
@@ -1582,24 +1983,48 @@
       <c r="K16">
         <v>9.3807644999999995E-2</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>-0.97261941619952719</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>-0.82897346551014106</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>-1.1155896963033207</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>-1.0664164875440196</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="7"/>
+        <v>-0.87882234485514577</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="8"/>
+        <v>0.34254988852028956</v>
+      </c>
+      <c r="R16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E17">
@@ -1623,24 +2048,48 @@
       <c r="K17">
         <v>0.150749261</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>-1.2559130983240685</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>-0.94335803600709145</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>-1.5652661873756246</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>-1.4065845282108524</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="7"/>
+        <v>-1.1052416684375066</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="8"/>
+        <v>0.69106965486483685</v>
+      </c>
+      <c r="R17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="C18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="D18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="E18">
@@ -1664,24 +2113,48 @@
       <c r="K18">
         <v>0.16465016199999999</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>-1.0901106377972924</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>-0.75359769937322074</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>-1.4229260154817736</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>-1.2547064056877</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="7"/>
+        <v>-0.9255148699067739</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="8"/>
+        <v>0.74590043703869457</v>
+      </c>
+      <c r="R18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="C19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="D19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E19">
@@ -1705,24 +2178,48 @@
       <c r="K19">
         <v>0.191645173</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>-2.5804286659588671</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>-2.3932333773633019</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>-2.7664328792222914</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>-2.7715984292372431</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="7"/>
+        <v>-2.3892589026807132</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="8"/>
+        <v>0.53428586145926538</v>
+      </c>
+      <c r="R19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
       <c r="B20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="C20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="D20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="E20">
@@ -1746,24 +2243,48 @@
       <c r="K20">
         <v>0.29794667699999999</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>-2.6128834182226335</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>-2.3210893589371562</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>-2.9017911985746991</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>-2.910075370646914</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="7"/>
+        <v>-2.3156914657982419</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="8"/>
+        <v>0.83096741987973388</v>
+      </c>
+      <c r="R20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="C21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="D21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E21">
@@ -1787,24 +2308,48 @@
       <c r="K21">
         <v>0.115620641</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>-1.1032342107845095</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>-0.99100574685273557</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>-1.2150486099988811</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>-1.2188209203726208</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="7"/>
+        <v>-0.98764750119628708</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="8"/>
+        <v>0.32192600743089922</v>
+      </c>
+      <c r="R21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
       <c r="B22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="C22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="E22">
@@ -1828,24 +2373,48 @@
       <c r="K22">
         <v>0.181507746</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>-1.3756108181480764</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>-1.1889039865727868</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
+        <v>-1.5611666477601815</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="6"/>
+        <v>-1.5569885894581859</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="7"/>
+        <v>-1.194233046838078</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="8"/>
+        <v>0.51977983090528823</v>
+      </c>
+      <c r="R22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
       <c r="B23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="C23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="D23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="E23">
@@ -1869,24 +2438,48 @@
       <c r="K23">
         <v>0.18763074499999999</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>-0.74894553676019271</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>-0.51431714003724593</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>-0.98178565157247544</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="6"/>
+        <v>-0.93661404163070117</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="7"/>
+        <v>-0.56127703188957323</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="8"/>
+        <v>0.59950369486632404</v>
+      </c>
+      <c r="R23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
       <c r="B24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="C24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="D24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E24">
@@ -1910,24 +2503,48 @@
       <c r="K24">
         <v>0.121956019</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>-0.76115221897399277</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>-0.64290339373018757</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>-0.87894507719399328</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>-0.88313251196081577</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="7"/>
+        <v>-0.63917192598716976</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="8"/>
+        <v>0.33945904589660325</v>
+      </c>
+      <c r="R24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
       <c r="B25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="D25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="E25">
@@ -1951,11 +2568,35 @@
       <c r="K25">
         <v>0.140033833</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>-1.0957730278233768</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>-0.8047959232999613</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="5"/>
+        <v>-1.3839816030206675</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>-1.2357612064236578</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="7"/>
+        <v>-0.95578484922298479</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="8"/>
+        <v>0.64330615742809061</v>
+      </c>
+      <c r="R25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1992,24 +2633,48 @@
       <c r="K26">
         <v>0.183176123</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>-2.5734550998482986</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>-2.3667463189790405</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>-2.7787321039690616</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="6"/>
+        <v>-2.7563335618593365</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="7"/>
+        <v>-2.3905766378373716</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="8"/>
+        <v>0.55091779287281439</v>
+      </c>
+      <c r="R26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:B37" si="6">IF(MOD(A27+4, 12)=0, 12, MOD(A27+4, 12))</f>
+        <f t="shared" ref="B27:B37" si="12">IF(MOD(A27+4, 12)=0, 12, MOD(A27+4, 12))</f>
         <v>6</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:C37" si="7">IF(MOD(A27+3, 12)=0, 12, MOD(A27+3, 12))</f>
+        <f t="shared" ref="C27:C37" si="13">IF(MOD(A27+3, 12)=0, 12, MOD(A27+3, 12))</f>
         <v>5</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:D37" si="8">IF(MOD(A27+2, 12)=0, 12, MOD(A27+2, 12))</f>
+        <f t="shared" ref="D27:D37" si="14">IF(MOD(A27+2, 12)=0, 12, MOD(A27+2, 12))</f>
         <v>4</v>
       </c>
       <c r="E27">
@@ -2033,24 +2698,48 @@
       <c r="K27">
         <v>0.19347826700000001</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27">
+        <f t="shared" si="3"/>
+        <v>-2.7201613193633678</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="4"/>
+        <v>-2.510812191251488</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>-2.9280355751729603</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="6"/>
+        <v>-2.9132735774394236</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="7"/>
+        <v>-2.527049061287201</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="8"/>
+        <v>0.56854615377109252</v>
+      </c>
+      <c r="R27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="C28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="D28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E28">
@@ -2074,24 +2763,48 @@
       <c r="K28">
         <v>0.23294488599999999</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28">
+        <f t="shared" si="3"/>
+        <v>-2.8712826735772801</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>-2.6008807301879378</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>-3.1392170056200319</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>-3.1037167641436714</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="7"/>
+        <v>-2.6388485830106667</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="8"/>
+        <v>0.71127236082671419</v>
+      </c>
+      <c r="R28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="C29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="D29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="E29">
@@ -2115,24 +2828,48 @@
       <c r="K29">
         <v>0.26151495299999999</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29">
+        <f t="shared" si="3"/>
+        <v>-2.9121241907973383</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="4"/>
+        <v>-2.6022372263013738</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>-3.2187656637707729</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="6"/>
+        <v>-3.1730210730617214</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="7"/>
+        <v>-2.6512273085329552</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="8"/>
+        <v>0.80769799238921003</v>
+      </c>
+      <c r="R29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="C30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="D30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E30">
@@ -2156,24 +2893,48 @@
       <c r="K30">
         <v>0.303454785</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30">
+        <f t="shared" si="3"/>
+        <v>-2.6927826105788144</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="4"/>
+        <v>-2.3567360476655086</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
+        <v>-3.0250479945203024</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="6"/>
+        <v>-2.9956777186525008</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="7"/>
+        <v>-2.389887502505128</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="8"/>
+        <v>0.9020103349123697</v>
+      </c>
+      <c r="R30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
       <c r="B31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="C31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="D31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="E31">
@@ -2197,24 +2958,48 @@
       <c r="K31">
         <v>0.41642526800000002</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31">
+        <f t="shared" si="3"/>
+        <v>-2.2152520076929028</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="4"/>
+        <v>-1.7851952131197057</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>-2.6392335522391619</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="6"/>
+        <v>-2.63132480851902</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="7"/>
+        <v>-1.7991792068667856</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="8"/>
+        <v>1.1924125909411887</v>
+      </c>
+      <c r="R31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
       <c r="B32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="C32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="D32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="E32">
@@ -2238,24 +3023,48 @@
       <c r="K32">
         <v>0.349941797</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L32">
+        <f t="shared" si="3"/>
+        <v>-2.1906063664279829</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="4"/>
+        <v>-1.8404201836104139</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>-2.5367585182126673</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="6"/>
+        <v>-2.5402781125790641</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="7"/>
+        <v>-1.8409346202769017</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="8"/>
+        <v>0.98689837190159779</v>
+      </c>
+      <c r="R32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
       <c r="B33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="C33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="D33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E33">
@@ -2279,24 +3088,48 @@
       <c r="K33">
         <v>0.32852886399999998</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33">
+        <f t="shared" si="3"/>
+        <v>-2.288491039738938</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="4"/>
+        <v>-1.8984008566831356</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>-2.6735607535379735</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="6"/>
+        <v>-2.6166783024557105</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="7"/>
+        <v>-1.9603037770220544</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="8"/>
+        <v>1.015726529795427</v>
+      </c>
+      <c r="R33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
       <c r="B34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="C34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="D34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="E34">
@@ -2320,24 +3153,48 @@
       <c r="K34">
         <v>0.258166638</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34">
+        <f t="shared" si="3"/>
+        <v>-2.2084567265910904</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="4"/>
+        <v>-1.9603314761822421</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>-2.4545499147335947</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="6"/>
+        <v>-2.4664246886081376</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="7"/>
+        <v>-1.9504887645740432</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="8"/>
+        <v>0.71445205767290776</v>
+      </c>
+      <c r="R34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10</v>
       </c>
       <c r="B35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="D35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="E35">
@@ -2361,24 +3218,48 @@
       <c r="K35">
         <v>0.41170104899999999</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L35">
+        <f t="shared" si="3"/>
+        <v>-1.8242394616828639</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="4"/>
+        <v>-1.3752962660653623</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="5"/>
+        <v>-2.2666524729691995</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="6"/>
+        <v>-2.2359346376513711</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="7"/>
+        <v>-1.4125442857143566</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="8"/>
+        <v>1.2134609838181682</v>
+      </c>
+      <c r="R35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
       <c r="B36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="C36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="D36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E36">
@@ -2402,24 +3283,48 @@
       <c r="K36">
         <v>0.27103965400000002</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L36">
+        <f t="shared" si="3"/>
+        <v>-1.8599602513803548</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="4"/>
+        <v>-1.5593797154336286</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>-2.1575940453918419</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="6"/>
+        <v>-2.1309646199548782</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="7"/>
+        <v>-1.5889558828057204</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="8"/>
+        <v>0.80723841318000888</v>
+      </c>
+      <c r="R36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12</v>
       </c>
       <c r="B37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="C37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="D37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E37">
@@ -2443,7 +3348,31 @@
       <c r="K37">
         <v>0.22612389099999999</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37">
+        <f t="shared" si="3"/>
+        <v>-2.3223208886681279</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="4"/>
+        <v>-2.073796697871888</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="5"/>
+        <v>-2.5687966143665975</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="6"/>
+        <v>-2.5482019988203319</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="7"/>
+        <v>-2.0964397785159239</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="8"/>
+        <v>0.67015969814973042</v>
+      </c>
+      <c r="R37" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>